<commit_message>
idek a ton of stuff
</commit_message>
<xml_diff>
--- a/Variable Notes.xlsx
+++ b/Variable Notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="560" windowWidth="18240" windowHeight="20060" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="540" windowWidth="18240" windowHeight="20060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -927,131 +927,130 @@
   </si>
   <si>
     <r>
+      <t>PoolArea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Pool area in square feet </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Fence quality </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MiscFeature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Miscellaneous feature not covered in other categories </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MiscVal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: $Value of miscellaneous feature </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MoSold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Month Sold </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>YrSold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Year Sold </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SaleType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Type of sale </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SaleCondition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF44474C"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Condition of sale </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PoolQC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">: Pool quality </t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>ScreenPorch</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF44474C"/>
         <rFont val="ArialMT"/>
       </rPr>
       <t xml:space="preserve">: Screen porch area in square feet </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PoolArea</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Pool area in square feet </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fence</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Fence quality </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MiscFeature</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Miscellaneous feature not covered in other categories </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MiscVal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: $Value of miscellaneous feature </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>MoSold</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Month Sold </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>YrSold</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Year Sold </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SaleType</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Type of sale </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SaleCondition</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF44474C"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Condition of sale </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>PoolQC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">: Pool quality </t>
     </r>
   </si>
 </sst>
@@ -1092,7 +1091,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1123,6 +1122,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1136,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1149,6 +1154,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1542,13 +1551,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1562,8 +1571,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1582,13 +1591,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1597,8 +1606,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1622,13 +1631,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1642,13 +1651,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1662,8 +1671,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1677,8 +1686,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1687,8 +1696,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1702,8 +1711,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1722,8 +1731,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1737,23 +1746,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1782,54 +1791,54 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="14" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="10" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>